<commit_message>
Working on UI sorry if its a lil ugly rn
</commit_message>
<xml_diff>
--- a/Track_Model/Green Line.xlsx
+++ b/Track_Model/Green Line.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DRich\PycharmProjects\ece1140-tovarish\Track_Model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DRich\PycharmProjects\ece1140-tovarish\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CEBF91C-2365-44A7-B0A0-E6AE71C55CD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB616C5E-E650-43E5-BF30-4B680655276A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{12A04384-6BD8-4EE6-B8F6-E9FF68EB782F}"/>
+    <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="13770" xr2:uid="{12A04384-6BD8-4EE6-B8F6-E9FF68EB782F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="108">
   <si>
     <t>Line</t>
   </si>
@@ -188,9 +188,6 @@
     <t>Beacon Message</t>
   </si>
   <si>
-    <t>Beacon Msg Here</t>
-  </si>
-  <si>
     <t>SWITCH (28-29, 150-28)</t>
   </si>
   <si>
@@ -219,6 +216,150 @@
   </si>
   <si>
     <t>SWITCH (13-12, 1-13)</t>
+  </si>
+  <si>
+    <t>G100</t>
+  </si>
+  <si>
+    <t>G101</t>
+  </si>
+  <si>
+    <t>G104</t>
+  </si>
+  <si>
+    <t>G106</t>
+  </si>
+  <si>
+    <t>G113</t>
+  </si>
+  <si>
+    <t>G115</t>
+  </si>
+  <si>
+    <t>G122</t>
+  </si>
+  <si>
+    <t>G124</t>
+  </si>
+  <si>
+    <t>G131</t>
+  </si>
+  <si>
+    <t>G133</t>
+  </si>
+  <si>
+    <t>G140</t>
+  </si>
+  <si>
+    <t>G142</t>
+  </si>
+  <si>
+    <t>G150</t>
+  </si>
+  <si>
+    <t>G001</t>
+  </si>
+  <si>
+    <t>G003</t>
+  </si>
+  <si>
+    <t>G008</t>
+  </si>
+  <si>
+    <t>G010</t>
+  </si>
+  <si>
+    <t>G012</t>
+  </si>
+  <si>
+    <t>G013</t>
+  </si>
+  <si>
+    <t>G015</t>
+  </si>
+  <si>
+    <t>G017</t>
+  </si>
+  <si>
+    <t>G021</t>
+  </si>
+  <si>
+    <t>G023</t>
+  </si>
+  <si>
+    <t>G028</t>
+  </si>
+  <si>
+    <t>G029</t>
+  </si>
+  <si>
+    <t>G030</t>
+  </si>
+  <si>
+    <t>G032</t>
+  </si>
+  <si>
+    <t>G038</t>
+  </si>
+  <si>
+    <t>G040</t>
+  </si>
+  <si>
+    <t>G047</t>
+  </si>
+  <si>
+    <t>G049</t>
+  </si>
+  <si>
+    <t>G056</t>
+  </si>
+  <si>
+    <t>G057</t>
+  </si>
+  <si>
+    <t>G058</t>
+  </si>
+  <si>
+    <t>G063</t>
+  </si>
+  <si>
+    <t>G064</t>
+  </si>
+  <si>
+    <t>G066</t>
+  </si>
+  <si>
+    <t>G072</t>
+  </si>
+  <si>
+    <t>G074</t>
+  </si>
+  <si>
+    <t>G076</t>
+  </si>
+  <si>
+    <t>G077</t>
+  </si>
+  <si>
+    <t>G078</t>
+  </si>
+  <si>
+    <t>G085</t>
+  </si>
+  <si>
+    <t>G086</t>
+  </si>
+  <si>
+    <t>G087</t>
+  </si>
+  <si>
+    <t>G089</t>
+  </si>
+  <si>
+    <t>G095</t>
+  </si>
+  <si>
+    <t>G097</t>
   </si>
 </sst>
 </file>
@@ -645,28 +786,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F25EB9E2-F902-42D7-8339-00ED3A2A22AE}">
   <dimension ref="A1:L151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="C102" sqref="C102"/>
+    <sheetView tabSelected="1" topLeftCell="B114" workbookViewId="0">
+      <selection activeCell="J131" sqref="J131"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.54296875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.1796875" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.1796875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.54296875" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.54296875" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" style="8" customWidth="1"/>
-    <col min="8" max="8" width="23.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.42578125" style="8" customWidth="1"/>
-    <col min="11" max="11" width="8.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="8"/>
+    <col min="8" max="8" width="23.453125" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.81640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.453125" style="8" customWidth="1"/>
+    <col min="11" max="11" width="8.54296875" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.1796875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="63" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="48" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -700,7 +841,7 @@
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
     </row>
-    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -725,12 +866,12 @@
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="9" t="s">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="K2" s="4"/>
       <c r="L2" s="6"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="str">
         <f>A2</f>
         <v>Green</v>
@@ -763,7 +904,7 @@
       <c r="K3" s="4"/>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="str">
         <f t="shared" ref="A4:A67" si="0">A3</f>
         <v>Green</v>
@@ -789,12 +930,12 @@
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="9" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="K4" s="4"/>
       <c r="L4" s="6"/>
     </row>
-    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -823,7 +964,7 @@
       <c r="K5" s="4"/>
       <c r="L5" s="6"/>
     </row>
-    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -852,7 +993,7 @@
       <c r="K6" s="4"/>
       <c r="L6" s="6"/>
     </row>
-    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -881,7 +1022,7 @@
       <c r="K7" s="4"/>
       <c r="L7" s="6"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -910,7 +1051,7 @@
       <c r="K8" s="4"/>
       <c r="L8" s="6"/>
     </row>
-    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -936,12 +1077,12 @@
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="9" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="K9" s="4"/>
       <c r="L9" s="6"/>
     </row>
-    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A10" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -974,7 +1115,7 @@
       <c r="K10" s="4"/>
       <c r="L10" s="6"/>
     </row>
-    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -1000,12 +1141,12 @@
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="9" t="s">
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="K11" s="4"/>
       <c r="L11" s="6"/>
     </row>
-    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A12" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -1034,7 +1175,7 @@
       <c r="K12" s="4"/>
       <c r="L12" s="6"/>
     </row>
-    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A13" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -1059,11 +1200,13 @@
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
+      <c r="J13" s="4" t="s">
+        <v>77</v>
+      </c>
       <c r="K13" s="4"/>
       <c r="L13" s="6"/>
     </row>
-    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A14" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -1087,14 +1230,16 @@
         <v>0.5</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
+      <c r="J14" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="K14" s="4"/>
       <c r="L14" s="6"/>
     </row>
-    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A15" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -1123,7 +1268,7 @@
       <c r="K15" s="4"/>
       <c r="L15" s="6"/>
     </row>
-    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A16" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -1149,12 +1294,12 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="9" t="s">
-        <v>50</v>
+        <v>79</v>
       </c>
       <c r="K16" s="4"/>
       <c r="L16" s="6"/>
     </row>
-    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A17" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -1178,16 +1323,16 @@
         <v>0.5</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
       <c r="L17" s="6"/>
     </row>
-    <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A18" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -1213,12 +1358,12 @@
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="J18" s="9" t="s">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="K18" s="4"/>
       <c r="L18" s="6"/>
     </row>
-    <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A19" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -1247,7 +1392,7 @@
       <c r="K19" s="4"/>
       <c r="L19" s="6"/>
     </row>
-    <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A20" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -1278,7 +1423,7 @@
       <c r="K20" s="4"/>
       <c r="L20" s="6"/>
     </row>
-    <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A21" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -1307,7 +1452,7 @@
       <c r="K21" s="4"/>
       <c r="L21" s="6"/>
     </row>
-    <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A22" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -1333,12 +1478,12 @@
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="J22" s="9" t="s">
-        <v>50</v>
+        <v>81</v>
       </c>
       <c r="K22" s="4"/>
       <c r="L22" s="6"/>
     </row>
-    <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A23" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -1365,13 +1510,13 @@
         <v>41</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
       <c r="L23" s="6"/>
     </row>
-    <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A24" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -1397,12 +1542,12 @@
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
       <c r="J24" s="9" t="s">
-        <v>50</v>
+        <v>82</v>
       </c>
       <c r="K24" s="4"/>
       <c r="L24" s="6"/>
     </row>
-    <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A25" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -1431,7 +1576,7 @@
       <c r="K25" s="4"/>
       <c r="L25" s="6"/>
     </row>
-    <row r="26" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A26" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -1460,7 +1605,7 @@
       <c r="K26" s="4"/>
       <c r="L26" s="6"/>
     </row>
-    <row r="27" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A27" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -1489,7 +1634,7 @@
       <c r="K27" s="4"/>
       <c r="L27" s="6"/>
     </row>
-    <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A28" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -1518,7 +1663,7 @@
       <c r="K28" s="4"/>
       <c r="L28" s="6"/>
     </row>
-    <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A29" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -1542,14 +1687,16 @@
         <v>0.5</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
+      <c r="J29" s="4" t="s">
+        <v>83</v>
+      </c>
       <c r="K29" s="4"/>
       <c r="L29" s="6"/>
     </row>
-    <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A30" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -1574,11 +1721,13 @@
       </c>
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
+      <c r="J30" s="4" t="s">
+        <v>84</v>
+      </c>
       <c r="K30" s="4"/>
       <c r="L30" s="6"/>
     </row>
-    <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A31" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -1604,12 +1753,12 @@
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
       <c r="J31" s="9" t="s">
-        <v>50</v>
+        <v>85</v>
       </c>
       <c r="K31" s="4"/>
       <c r="L31" s="6"/>
     </row>
-    <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A32" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -1642,7 +1791,7 @@
       <c r="K32" s="4"/>
       <c r="L32" s="6"/>
     </row>
-    <row r="33" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A33" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -1668,12 +1817,12 @@
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
       <c r="J33" s="9" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="K33" s="4"/>
       <c r="L33" s="6"/>
     </row>
-    <row r="34" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A34" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -1702,7 +1851,7 @@
       <c r="K34" s="4"/>
       <c r="L34" s="6"/>
     </row>
-    <row r="35" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A35" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -1731,7 +1880,7 @@
       <c r="K35" s="4"/>
       <c r="L35" s="6"/>
     </row>
-    <row r="36" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A36" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -1760,7 +1909,7 @@
       <c r="K36" s="4"/>
       <c r="L36" s="6"/>
     </row>
-    <row r="37" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A37" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -1791,7 +1940,7 @@
       <c r="K37" s="4"/>
       <c r="L37" s="6"/>
     </row>
-    <row r="38" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A38" s="4" t="str">
         <f>A34</f>
         <v>Green</v>
@@ -1822,7 +1971,7 @@
       <c r="K38" s="4"/>
       <c r="L38" s="6"/>
     </row>
-    <row r="39" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A39" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -1850,12 +1999,12 @@
       </c>
       <c r="I39" s="4"/>
       <c r="J39" s="9" t="s">
-        <v>50</v>
+        <v>87</v>
       </c>
       <c r="K39" s="4"/>
       <c r="L39" s="6"/>
     </row>
-    <row r="40" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" ht="32" x14ac:dyDescent="0.4">
       <c r="A40" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -1879,7 +2028,7 @@
         <v>0.5</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I40" s="4" t="s">
         <v>21</v>
@@ -1888,7 +2037,7 @@
       <c r="K40" s="4"/>
       <c r="L40" s="6"/>
     </row>
-    <row r="41" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A41" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -1916,12 +2065,12 @@
       </c>
       <c r="I41" s="4"/>
       <c r="J41" s="9" t="s">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="K41" s="4"/>
       <c r="L41" s="6"/>
     </row>
-    <row r="42" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A42" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -1952,7 +2101,7 @@
       <c r="K42" s="4"/>
       <c r="L42" s="6"/>
     </row>
-    <row r="43" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A43" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -1983,7 +2132,7 @@
       <c r="K43" s="4"/>
       <c r="L43" s="6"/>
     </row>
-    <row r="44" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A44" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -2014,7 +2163,7 @@
       <c r="K44" s="4"/>
       <c r="L44" s="6"/>
     </row>
-    <row r="45" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A45" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -2045,7 +2194,7 @@
       <c r="K45" s="4"/>
       <c r="L45" s="6"/>
     </row>
-    <row r="46" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A46" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -2076,7 +2225,7 @@
       <c r="K46" s="4"/>
       <c r="L46" s="6"/>
     </row>
-    <row r="47" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A47" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -2107,7 +2256,7 @@
       <c r="K47" s="4"/>
       <c r="L47" s="6"/>
     </row>
-    <row r="48" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A48" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -2135,12 +2284,12 @@
       </c>
       <c r="I48" s="4"/>
       <c r="J48" s="9" t="s">
-        <v>50</v>
+        <v>89</v>
       </c>
       <c r="K48" s="4"/>
       <c r="L48" s="6"/>
     </row>
-    <row r="49" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" ht="32" x14ac:dyDescent="0.4">
       <c r="A49" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -2173,7 +2322,7 @@
       <c r="K49" s="4"/>
       <c r="L49" s="6"/>
     </row>
-    <row r="50" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A50" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -2201,12 +2350,12 @@
       </c>
       <c r="I50" s="4"/>
       <c r="J50" s="9" t="s">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="K50" s="4"/>
       <c r="L50" s="6"/>
     </row>
-    <row r="51" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A51" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -2237,7 +2386,7 @@
       <c r="K51" s="4"/>
       <c r="L51" s="6"/>
     </row>
-    <row r="52" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A52" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -2268,7 +2417,7 @@
       <c r="K52" s="4"/>
       <c r="L52" s="6"/>
     </row>
-    <row r="53" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A53" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -2299,7 +2448,7 @@
       <c r="K53" s="4"/>
       <c r="L53" s="6"/>
     </row>
-    <row r="54" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A54" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -2330,7 +2479,7 @@
       <c r="K54" s="4"/>
       <c r="L54" s="6"/>
     </row>
-    <row r="55" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A55" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -2361,7 +2510,7 @@
       <c r="K55" s="4"/>
       <c r="L55" s="6"/>
     </row>
-    <row r="56" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A56" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -2392,7 +2541,7 @@
       <c r="K56" s="4"/>
       <c r="L56" s="6"/>
     </row>
-    <row r="57" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A57" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -2420,12 +2569,12 @@
       </c>
       <c r="I57" s="4"/>
       <c r="J57" s="9" t="s">
-        <v>50</v>
+        <v>91</v>
       </c>
       <c r="K57" s="4"/>
       <c r="L57" s="6"/>
     </row>
-    <row r="58" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" ht="48" x14ac:dyDescent="0.4">
       <c r="A58" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -2449,16 +2598,18 @@
         <v>0.5</v>
       </c>
       <c r="H58" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I58" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J58" s="4"/>
+      <c r="J58" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="K58" s="4"/>
       <c r="L58" s="6"/>
     </row>
-    <row r="59" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A59" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -2484,12 +2635,12 @@
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
       <c r="J59" s="9" t="s">
-        <v>50</v>
+        <v>93</v>
       </c>
       <c r="K59" s="4"/>
       <c r="L59" s="6"/>
     </row>
-    <row r="60" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A60" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -2517,7 +2668,7 @@
       <c r="K60" s="4"/>
       <c r="L60" s="6"/>
     </row>
-    <row r="61" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A61" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -2546,7 +2697,7 @@
       <c r="K61" s="4"/>
       <c r="L61" s="6"/>
     </row>
-    <row r="62" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A62" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -2575,7 +2726,7 @@
       <c r="K62" s="4"/>
       <c r="L62" s="6"/>
     </row>
-    <row r="63" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A63" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -2604,7 +2755,7 @@
       <c r="K63" s="4"/>
       <c r="L63" s="6"/>
     </row>
-    <row r="64" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A64" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -2628,14 +2779,16 @@
         <v>0.5</v>
       </c>
       <c r="H64" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I64" s="4"/>
-      <c r="J64" s="4"/>
+      <c r="J64" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="K64" s="4"/>
       <c r="L64" s="6"/>
     </row>
-    <row r="65" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A65" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -2660,11 +2813,13 @@
       </c>
       <c r="H65" s="4"/>
       <c r="I65" s="4"/>
-      <c r="J65" s="4"/>
+      <c r="J65" s="4" t="s">
+        <v>95</v>
+      </c>
       <c r="K65" s="4"/>
       <c r="L65" s="6"/>
     </row>
-    <row r="66" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A66" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -2697,7 +2852,7 @@
       <c r="K66" s="4"/>
       <c r="L66" s="6"/>
     </row>
-    <row r="67" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A67" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
@@ -2722,11 +2877,13 @@
       </c>
       <c r="H67" s="4"/>
       <c r="I67" s="4"/>
-      <c r="J67" s="4"/>
+      <c r="J67" s="4" t="s">
+        <v>96</v>
+      </c>
       <c r="K67" s="4"/>
       <c r="L67" s="6"/>
     </row>
-    <row r="68" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A68" s="4" t="str">
         <f t="shared" ref="A68:A131" si="1">A67</f>
         <v>Green</v>
@@ -2755,7 +2912,7 @@
       <c r="K68" s="4"/>
       <c r="L68" s="6"/>
     </row>
-    <row r="69" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A69" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -2784,7 +2941,7 @@
       <c r="K69" s="4"/>
       <c r="L69" s="6"/>
     </row>
-    <row r="70" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A70" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -2813,7 +2970,7 @@
       <c r="K70" s="4"/>
       <c r="L70" s="6"/>
     </row>
-    <row r="71" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A71" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -2842,7 +2999,7 @@
       <c r="K71" s="4"/>
       <c r="L71" s="6"/>
     </row>
-    <row r="72" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A72" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -2871,7 +3028,7 @@
       <c r="K72" s="4"/>
       <c r="L72" s="6"/>
     </row>
-    <row r="73" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A73" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -2897,12 +3054,12 @@
       <c r="H73" s="4"/>
       <c r="I73" s="4"/>
       <c r="J73" s="9" t="s">
-        <v>50</v>
+        <v>97</v>
       </c>
       <c r="K73" s="4"/>
       <c r="L73" s="6"/>
     </row>
-    <row r="74" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A74" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -2935,7 +3092,7 @@
       <c r="K74" s="4"/>
       <c r="L74" s="6"/>
     </row>
-    <row r="75" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A75" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -2961,12 +3118,12 @@
       <c r="H75" s="4"/>
       <c r="I75" s="4"/>
       <c r="J75" s="9" t="s">
-        <v>50</v>
+        <v>98</v>
       </c>
       <c r="K75" s="4"/>
       <c r="L75" s="6"/>
     </row>
-    <row r="76" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A76" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -2995,7 +3152,7 @@
       <c r="K76" s="4"/>
       <c r="L76" s="6"/>
     </row>
-    <row r="77" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A77" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3021,12 +3178,12 @@
       <c r="H77" s="4"/>
       <c r="I77" s="4"/>
       <c r="J77" s="9" t="s">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="K77" s="4"/>
       <c r="L77" s="6"/>
     </row>
-    <row r="78" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" ht="32" x14ac:dyDescent="0.4">
       <c r="A78" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3050,16 +3207,18 @@
         <v>0.5</v>
       </c>
       <c r="H78" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I78" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="I78" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="J78" s="4"/>
+      <c r="J78" s="4" t="s">
+        <v>100</v>
+      </c>
       <c r="K78" s="4"/>
       <c r="L78" s="6"/>
     </row>
-    <row r="79" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A79" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3085,12 +3244,12 @@
       <c r="H79" s="4"/>
       <c r="I79" s="4"/>
       <c r="J79" s="9" t="s">
-        <v>50</v>
+        <v>101</v>
       </c>
       <c r="K79" s="4"/>
       <c r="L79" s="6"/>
     </row>
-    <row r="80" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A80" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3119,7 +3278,7 @@
       <c r="K80" s="4"/>
       <c r="L80" s="6"/>
     </row>
-    <row r="81" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A81" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3148,7 +3307,7 @@
       <c r="K81" s="4"/>
       <c r="L81" s="6"/>
     </row>
-    <row r="82" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A82" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3177,7 +3336,7 @@
       <c r="K82" s="4"/>
       <c r="L82" s="6"/>
     </row>
-    <row r="83" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A83" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3206,7 +3365,7 @@
       <c r="K83" s="4"/>
       <c r="L83" s="6"/>
     </row>
-    <row r="84" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A84" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3235,7 +3394,7 @@
       <c r="K84" s="4"/>
       <c r="L84" s="6"/>
     </row>
-    <row r="85" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A85" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3264,7 +3423,7 @@
       <c r="K85" s="4"/>
       <c r="L85" s="6"/>
     </row>
-    <row r="86" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A86" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3288,14 +3447,16 @@
         <v>0.5</v>
       </c>
       <c r="H86" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I86" s="4"/>
-      <c r="J86" s="4"/>
+      <c r="J86" s="4" t="s">
+        <v>102</v>
+      </c>
       <c r="K86" s="4"/>
       <c r="L86" s="6"/>
     </row>
-    <row r="87" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A87" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3320,11 +3481,13 @@
       </c>
       <c r="H87" s="4"/>
       <c r="I87" s="4"/>
-      <c r="J87" s="4"/>
+      <c r="J87" s="4" t="s">
+        <v>103</v>
+      </c>
       <c r="K87" s="4"/>
       <c r="L87" s="6"/>
     </row>
-    <row r="88" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A88" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3350,12 +3513,12 @@
       <c r="H88" s="4"/>
       <c r="I88" s="4"/>
       <c r="J88" s="9" t="s">
-        <v>50</v>
+        <v>104</v>
       </c>
       <c r="K88" s="4"/>
       <c r="L88" s="6"/>
     </row>
-    <row r="89" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A89" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3388,7 +3551,7 @@
       <c r="K89" s="4"/>
       <c r="L89" s="6"/>
     </row>
-    <row r="90" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A90" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3414,12 +3577,12 @@
       <c r="H90" s="4"/>
       <c r="I90" s="4"/>
       <c r="J90" s="9" t="s">
-        <v>50</v>
+        <v>105</v>
       </c>
       <c r="K90" s="4"/>
       <c r="L90" s="6"/>
     </row>
-    <row r="91" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A91" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3448,7 +3611,7 @@
       <c r="K91" s="4"/>
       <c r="L91" s="6"/>
     </row>
-    <row r="92" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A92" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3477,7 +3640,7 @@
       <c r="K92" s="4"/>
       <c r="L92" s="6"/>
     </row>
-    <row r="93" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A93" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3506,7 +3669,7 @@
       <c r="K93" s="4"/>
       <c r="L93" s="6"/>
     </row>
-    <row r="94" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A94" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3535,7 +3698,7 @@
       <c r="K94" s="4"/>
       <c r="L94" s="6"/>
     </row>
-    <row r="95" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A95" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3564,7 +3727,7 @@
       <c r="K95" s="4"/>
       <c r="L95" s="6"/>
     </row>
-    <row r="96" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A96" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3590,12 +3753,12 @@
       <c r="H96" s="4"/>
       <c r="I96" s="4"/>
       <c r="J96" s="9" t="s">
-        <v>50</v>
+        <v>106</v>
       </c>
       <c r="K96" s="4"/>
       <c r="L96" s="6"/>
     </row>
-    <row r="97" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" ht="32" x14ac:dyDescent="0.4">
       <c r="A97" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3628,7 +3791,7 @@
       <c r="K97" s="4"/>
       <c r="L97" s="6"/>
     </row>
-    <row r="98" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A98" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3654,12 +3817,12 @@
       <c r="H98" s="4"/>
       <c r="I98" s="4"/>
       <c r="J98" s="9" t="s">
-        <v>50</v>
+        <v>107</v>
       </c>
       <c r="K98" s="4"/>
       <c r="L98" s="6"/>
     </row>
-    <row r="99" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A99" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3688,7 +3851,7 @@
       <c r="K99" s="4"/>
       <c r="L99" s="6"/>
     </row>
-    <row r="100" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A100" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3717,7 +3880,7 @@
       <c r="K100" s="4"/>
       <c r="L100" s="6"/>
     </row>
-    <row r="101" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A101" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3742,11 +3905,13 @@
       </c>
       <c r="H101" s="4"/>
       <c r="I101" s="4"/>
-      <c r="J101" s="4"/>
+      <c r="J101" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="K101" s="4"/>
       <c r="L101" s="6"/>
     </row>
-    <row r="102" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A102" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3771,11 +3936,13 @@
       </c>
       <c r="H102" s="4"/>
       <c r="I102" s="4"/>
-      <c r="J102" s="4"/>
+      <c r="J102" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="K102" s="4"/>
       <c r="L102" s="6"/>
     </row>
-    <row r="103" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A103" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3804,7 +3971,7 @@
       <c r="K103" s="4"/>
       <c r="L103" s="6"/>
     </row>
-    <row r="104" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A104" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3833,7 +4000,7 @@
       <c r="K104" s="4"/>
       <c r="L104" s="6"/>
     </row>
-    <row r="105" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A105" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3859,12 +4026,12 @@
       <c r="H105" s="4"/>
       <c r="I105" s="4"/>
       <c r="J105" s="9" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="K105" s="4"/>
       <c r="L105" s="6"/>
     </row>
-    <row r="106" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A106" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3898,7 +4065,7 @@
       <c r="K106" s="4"/>
       <c r="L106" s="6"/>
     </row>
-    <row r="107" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A107" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3924,12 +4091,12 @@
       <c r="H107" s="4"/>
       <c r="I107" s="4"/>
       <c r="J107" s="9" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="K107" s="4"/>
       <c r="L107" s="6"/>
     </row>
-    <row r="108" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A108" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3958,7 +4125,7 @@
       <c r="K108" s="4"/>
       <c r="L108" s="6"/>
     </row>
-    <row r="109" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A109" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3989,7 +4156,7 @@
       <c r="K109" s="4"/>
       <c r="L109" s="6"/>
     </row>
-    <row r="110" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A110" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4018,7 +4185,7 @@
       <c r="K110" s="4"/>
       <c r="L110" s="6"/>
     </row>
-    <row r="111" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A111" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4047,7 +4214,7 @@
       <c r="K111" s="4"/>
       <c r="L111" s="6"/>
     </row>
-    <row r="112" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A112" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4076,7 +4243,7 @@
       <c r="K112" s="4"/>
       <c r="L112" s="6"/>
     </row>
-    <row r="113" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A113" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4105,7 +4272,7 @@
       <c r="K113" s="4"/>
       <c r="L113" s="6"/>
     </row>
-    <row r="114" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A114" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4131,12 +4298,12 @@
       <c r="H114" s="4"/>
       <c r="I114" s="4"/>
       <c r="J114" s="9" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="K114" s="4"/>
       <c r="L114" s="6"/>
     </row>
-    <row r="115" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A115" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4171,7 +4338,7 @@
       <c r="K115" s="4"/>
       <c r="L115" s="6"/>
     </row>
-    <row r="116" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A116" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4197,12 +4364,12 @@
       <c r="H116" s="4"/>
       <c r="I116" s="4"/>
       <c r="J116" s="9" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="K116" s="4"/>
       <c r="L116" s="6"/>
     </row>
-    <row r="117" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A117" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4231,7 +4398,7 @@
       <c r="K117" s="4"/>
       <c r="L117" s="6"/>
     </row>
-    <row r="118" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A118" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4260,7 +4427,7 @@
       <c r="K118" s="4"/>
       <c r="L118" s="6"/>
     </row>
-    <row r="119" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A119" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4289,7 +4456,7 @@
       <c r="K119" s="4"/>
       <c r="L119" s="6"/>
     </row>
-    <row r="120" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A120" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4318,7 +4485,7 @@
       <c r="K120" s="4"/>
       <c r="L120" s="6"/>
     </row>
-    <row r="121" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A121" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4347,7 +4514,7 @@
       <c r="K121" s="4"/>
       <c r="L121" s="6"/>
     </row>
-    <row r="122" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A122" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4376,7 +4543,7 @@
       <c r="K122" s="4"/>
       <c r="L122" s="6"/>
     </row>
-    <row r="123" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A123" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4404,12 +4571,12 @@
       </c>
       <c r="I123" s="4"/>
       <c r="J123" s="9" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="K123" s="4"/>
       <c r="L123" s="6"/>
     </row>
-    <row r="124" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" ht="32" x14ac:dyDescent="0.4">
       <c r="A124" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4433,7 +4600,7 @@
         <v>0.5</v>
       </c>
       <c r="H124" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I124" s="4" t="s">
         <v>21</v>
@@ -4442,7 +4609,7 @@
       <c r="K124" s="4"/>
       <c r="L124" s="6"/>
     </row>
-    <row r="125" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A125" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4470,12 +4637,12 @@
       </c>
       <c r="I125" s="4"/>
       <c r="J125" s="9" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="K125" s="4"/>
       <c r="L125" s="6"/>
     </row>
-    <row r="126" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A126" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4506,7 +4673,7 @@
       <c r="K126" s="4"/>
       <c r="L126" s="6"/>
     </row>
-    <row r="127" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A127" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4537,7 +4704,7 @@
       <c r="K127" s="4"/>
       <c r="L127" s="6"/>
     </row>
-    <row r="128" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A128" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4568,7 +4735,7 @@
       <c r="K128" s="4"/>
       <c r="L128" s="6"/>
     </row>
-    <row r="129" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A129" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4599,7 +4766,7 @@
       <c r="K129" s="4"/>
       <c r="L129" s="6"/>
     </row>
-    <row r="130" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A130" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4630,7 +4797,7 @@
       <c r="K130" s="4"/>
       <c r="L130" s="6"/>
     </row>
-    <row r="131" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A131" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4661,7 +4828,7 @@
       <c r="K131" s="4"/>
       <c r="L131" s="6"/>
     </row>
-    <row r="132" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A132" s="4" t="str">
         <f t="shared" ref="A132:A151" si="2">A131</f>
         <v>Green</v>
@@ -4689,12 +4856,12 @@
       </c>
       <c r="I132" s="4"/>
       <c r="J132" s="9" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="K132" s="4"/>
       <c r="L132" s="6"/>
     </row>
-    <row r="133" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" ht="32" x14ac:dyDescent="0.4">
       <c r="A133" s="4" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -4728,7 +4895,7 @@
       <c r="K133" s="4"/>
       <c r="L133" s="6"/>
     </row>
-    <row r="134" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A134" s="4" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -4756,12 +4923,12 @@
       </c>
       <c r="I134" s="4"/>
       <c r="J134" s="9" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="K134" s="4"/>
       <c r="L134" s="6"/>
     </row>
-    <row r="135" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A135" s="4" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -4792,7 +4959,7 @@
       <c r="K135" s="4"/>
       <c r="L135" s="6"/>
     </row>
-    <row r="136" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A136" s="4" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -4823,7 +4990,7 @@
       <c r="K136" s="4"/>
       <c r="L136" s="6"/>
     </row>
-    <row r="137" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A137" s="4" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -4854,7 +5021,7 @@
       <c r="K137" s="4"/>
       <c r="L137" s="6"/>
     </row>
-    <row r="138" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A138" s="4" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -4885,7 +5052,7 @@
       <c r="K138" s="4"/>
       <c r="L138" s="6"/>
     </row>
-    <row r="139" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A139" s="4" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -4916,7 +5083,7 @@
       <c r="K139" s="4"/>
       <c r="L139" s="6"/>
     </row>
-    <row r="140" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A140" s="4" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -4947,7 +5114,7 @@
       <c r="K140" s="4"/>
       <c r="L140" s="6"/>
     </row>
-    <row r="141" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A141" s="4" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -4975,12 +5142,12 @@
       </c>
       <c r="I141" s="4"/>
       <c r="J141" s="9" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="K141" s="4"/>
       <c r="L141" s="6"/>
     </row>
-    <row r="142" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:12" ht="32" x14ac:dyDescent="0.4">
       <c r="A142" s="4" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5014,7 +5181,7 @@
       <c r="K142" s="4"/>
       <c r="L142" s="6"/>
     </row>
-    <row r="143" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A143" s="4" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5042,12 +5209,12 @@
       </c>
       <c r="I143" s="4"/>
       <c r="J143" s="9" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="K143" s="4"/>
       <c r="L143" s="6"/>
     </row>
-    <row r="144" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A144" s="4" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5078,7 +5245,7 @@
       <c r="K144" s="4"/>
       <c r="L144" s="6"/>
     </row>
-    <row r="145" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A145" s="4" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5107,7 +5274,7 @@
       <c r="K145" s="4"/>
       <c r="L145" s="6"/>
     </row>
-    <row r="146" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A146" s="4" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5136,7 +5303,7 @@
       <c r="K146" s="4"/>
       <c r="L146" s="6"/>
     </row>
-    <row r="147" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A147" s="4" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5165,7 +5332,7 @@
       <c r="K147" s="4"/>
       <c r="L147" s="6"/>
     </row>
-    <row r="148" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A148" s="4" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5194,7 +5361,7 @@
       <c r="K148" s="4"/>
       <c r="L148" s="6"/>
     </row>
-    <row r="149" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A149" s="4" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5224,7 +5391,7 @@
       <c r="K149" s="4"/>
       <c r="L149" s="6"/>
     </row>
-    <row r="150" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A150" s="4" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5253,7 +5420,7 @@
       <c r="K150" s="4"/>
       <c r="L150" s="6"/>
     </row>
-    <row r="151" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:12" ht="16" x14ac:dyDescent="0.4">
       <c r="A151" s="4" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5278,7 +5445,9 @@
       </c>
       <c r="H151" s="4"/>
       <c r="I151" s="4"/>
-      <c r="J151" s="4"/>
+      <c r="J151" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="K151" s="4"/>
       <c r="L151" s="6"/>
     </row>

</xml_diff>